<commit_message>
feat: agregar Nissan Pathfinder 3.5 2003‑240k km al catálogo y detalle
</commit_message>
<xml_diff>
--- a/public/autos/catalogo.xlsx
+++ b/public/autos/catalogo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11102"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11109"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cate/Desktop/Tlovendo/public/autos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{E736A1C6-E2C0-624B-8F31-03D0FA86FDF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{76D11CE7-A7FF-494E-8D97-6C451B06669F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="29400" windowHeight="17160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="194">
   <si>
     <t>Motor y rendimiento</t>
   </si>
@@ -371,6 +371,9 @@
   </si>
   <si>
     <t>6990000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nissan </t>
   </si>
   <si>
     <t>Frontal</t>
@@ -2159,20 +2162,36 @@
     </row>
     <row r="19" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1"/>
-      <c r="B19" s="5"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
+      <c r="B19" s="5">
+        <v>17</v>
+      </c>
+      <c r="C19" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="E19" s="5">
+        <v>2003</v>
+      </c>
       <c r="F19" s="5"/>
       <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
+      <c r="H19" s="5">
+        <v>240000</v>
+      </c>
       <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
-      <c r="K19" s="5"/>
+      <c r="J19" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="K19" s="7">
+        <v>10500000</v>
+      </c>
       <c r="L19" s="5"/>
       <c r="M19" s="5"/>
       <c r="N19" s="5"/>
-      <c r="O19" s="5"/>
+      <c r="O19" s="8">
+        <v>45780</v>
+      </c>
       <c r="P19" s="5"/>
       <c r="Q19" s="5"/>
       <c r="R19" s="5"/>
@@ -35669,19 +35688,19 @@
         <v>7</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
@@ -35717,19 +35736,19 @@
         <v>2024</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="G3" s="16" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="H3" s="15" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="J3" s="17" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="L3" s="1"/>
       <c r="M3" s="1"/>
@@ -35765,19 +35784,19 @@
         <v>2024</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="G4" s="15" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H4" s="15" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="K4" s="5"/>
       <c r="L4" s="1"/>
@@ -35814,19 +35833,19 @@
         <v>2022</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="G5" s="15" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="H5" s="15" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="K5" s="5"/>
       <c r="L5" s="1"/>
@@ -35863,19 +35882,19 @@
         <v>2018</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="G6" s="15" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="H6" s="15" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="K6" s="5"/>
       <c r="L6" s="1"/>
@@ -35912,19 +35931,19 @@
         <v>2016</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="G7" s="15" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="H7" s="15" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="1"/>
@@ -35961,19 +35980,19 @@
         <v>2013</v>
       </c>
       <c r="F8" s="15" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="G8" s="15" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="H8" s="15" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="J8" s="15" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="K8" s="5"/>
       <c r="L8" s="1"/>
@@ -36010,19 +36029,19 @@
         <v>2018</v>
       </c>
       <c r="F9" s="15" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="G9" s="15" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="H9" s="15" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="K9" s="5"/>
       <c r="L9" s="1"/>
@@ -36059,19 +36078,19 @@
         <v>2018</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="G10" s="15" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H10" s="15" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I10" s="15" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="K10" s="5"/>
       <c r="L10" s="1"/>
@@ -36108,19 +36127,19 @@
         <v>2016</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="G11" s="15" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="H11" s="15" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="J11" s="15" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="K11" s="5"/>
       <c r="L11" s="1"/>
@@ -36157,19 +36176,19 @@
         <v>2020</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="G12" s="15" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="H12" s="15" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="K12" s="5"/>
       <c r="L12" s="1"/>
@@ -36206,19 +36225,19 @@
         <v>2022</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="G13" s="15" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="H13" s="15" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="J13" s="15" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="1"/>
@@ -63953,17 +63972,17 @@
         <v>9</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D2" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F2" s="19" t="str">
         <f t="shared" ref="F2:F16" si="1">CONCATENATE(B2,"_",C2,D2)</f>
         <v>9_frontal.jpg</v>
       </c>
       <c r="G2" s="19" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -63975,17 +63994,17 @@
         <v>9</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D3" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F3" s="19" t="str">
         <f t="shared" si="1"/>
         <v>9_lateral.jpg</v>
       </c>
       <c r="G3" s="19" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -63997,17 +64016,17 @@
         <v>9</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D4" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F4" s="19" t="str">
         <f t="shared" si="1"/>
         <v>9_posterior.jpg</v>
       </c>
       <c r="G4" s="19" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -64019,17 +64038,17 @@
         <v>9</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D5" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F5" s="19" t="str">
         <f t="shared" si="1"/>
         <v>9_tablero.jpg</v>
       </c>
       <c r="G5" s="19" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -64041,17 +64060,17 @@
         <v>9</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D6" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F6" s="19" t="str">
         <f t="shared" si="1"/>
         <v>9_asientos.jpg</v>
       </c>
       <c r="G6" s="19" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -64063,17 +64082,17 @@
         <v>10</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D7" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F7" s="19" t="str">
         <f t="shared" si="1"/>
         <v>10_frontal.jpg</v>
       </c>
       <c r="G7" s="19" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -64085,17 +64104,17 @@
         <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D8" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F8" s="19" t="str">
         <f t="shared" si="1"/>
         <v>10_lateral.jpg</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -64107,17 +64126,17 @@
         <v>10</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D9" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F9" s="19" t="str">
         <f t="shared" si="1"/>
         <v>10_posterior.jpg</v>
       </c>
       <c r="G9" s="19" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -64129,17 +64148,17 @@
         <v>10</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D10" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F10" s="19" t="str">
         <f t="shared" si="1"/>
         <v>10_tablero.jpg</v>
       </c>
       <c r="G10" s="19" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -64151,17 +64170,17 @@
         <v>10</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D11" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F11" s="19" t="str">
         <f t="shared" si="1"/>
         <v>10_asientos.jpg</v>
       </c>
       <c r="G11" s="19" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -64173,17 +64192,17 @@
         <v>11</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>172</v>
+        <v>173</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F12" s="19" t="str">
         <f t="shared" si="1"/>
         <v>11_frontal.jpg</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -64195,17 +64214,17 @@
         <v>11</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="D13" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F13" s="19" t="str">
         <f t="shared" si="1"/>
         <v>11_lateral.jpg</v>
       </c>
       <c r="G13" s="19" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -64217,17 +64236,17 @@
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="D14" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F14" s="19" t="str">
         <f t="shared" si="1"/>
         <v>11_posterior.jpg</v>
       </c>
       <c r="G14" s="19" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -64239,17 +64258,17 @@
         <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="D15" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F15" s="19" t="str">
         <f t="shared" si="1"/>
         <v>11_tablero.jpg</v>
       </c>
       <c r="G15" s="19" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -64261,17 +64280,17 @@
         <v>11</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="D16" s="19" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="F16" s="19" t="str">
         <f t="shared" si="1"/>
         <v>11_asientos.jpg</v>
       </c>
       <c r="G16" s="19" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>

</xml_diff>